<commit_message>
- added category "limitation" to the sheet
</commit_message>
<xml_diff>
--- a/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
+++ b/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bt100472\Documents\Subversion Neu\publications\2017\TTC 2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bt110513\git\benchmarx\master\examples\familiestopersons\BenchmarxFamiliesToPersons\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26652" windowHeight="12960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26655" windowHeight="12960"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Forward Batch</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>False negative (unexpected failure)</t>
+  </si>
+  <si>
+    <t>Limitation (tool does not support certain features)</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +245,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -395,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -425,19 +434,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -720,16 +730,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
@@ -758,7 +768,7 @@
       <c r="Q3" s="17"/>
       <c r="R3" s="17"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
@@ -768,8 +778,8 @@
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="18"/>
       <c r="J4" s="20"/>
       <c r="K4" s="17"/>
@@ -781,7 +791,7 @@
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="9" t="s">
@@ -789,8 +799,8 @@
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="18"/>
       <c r="J5" s="20"/>
       <c r="K5" s="17"/>
@@ -802,7 +812,7 @@
       <c r="Q5" s="17"/>
       <c r="R5" s="17"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9" t="s">
@@ -810,8 +820,8 @@
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
       <c r="I6" s="18"/>
       <c r="J6" s="20"/>
       <c r="K6" s="17"/>
@@ -823,7 +833,7 @@
       <c r="Q6" s="17"/>
       <c r="R6" s="17"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
@@ -831,8 +841,8 @@
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="33"/>
       <c r="I7" s="18"/>
       <c r="J7" s="20"/>
       <c r="K7" s="17"/>
@@ -844,7 +854,7 @@
       <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="D8" s="9" t="s">
@@ -852,8 +862,8 @@
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="33"/>
       <c r="I8" s="18"/>
       <c r="J8" s="20"/>
       <c r="K8" s="17"/>
@@ -865,7 +875,7 @@
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9" t="s">
@@ -873,8 +883,8 @@
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
       <c r="I9" s="18"/>
       <c r="J9" s="20"/>
       <c r="K9" s="17"/>
@@ -886,7 +896,7 @@
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9" t="s">
@@ -894,8 +904,8 @@
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
       <c r="I10" s="18"/>
       <c r="J10" s="20"/>
       <c r="K10" s="17"/>
@@ -907,14 +917,14 @@
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="2"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
@@ -926,7 +936,7 @@
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
         <v>1</v>
       </c>
@@ -934,8 +944,8 @@
       <c r="D12" s="12"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35"/>
       <c r="I12" s="20"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
@@ -947,7 +957,7 @@
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="28" t="s">
         <v>16</v>
       </c>
@@ -957,8 +967,8 @@
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="18"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
@@ -970,7 +980,7 @@
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="12" t="s">
@@ -978,8 +988,8 @@
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="18"/>
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
@@ -991,7 +1001,7 @@
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="28" t="s">
         <v>18</v>
       </c>
@@ -1001,8 +1011,8 @@
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="21"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
       <c r="I15" s="18"/>
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
@@ -1014,7 +1024,7 @@
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="12" t="s">
@@ -1022,8 +1032,8 @@
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="18"/>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
@@ -1035,7 +1045,7 @@
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="12" t="s">
@@ -1043,8 +1053,8 @@
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="21"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
       <c r="I17" s="18"/>
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
@@ -1056,7 +1066,7 @@
       <c r="Q17" s="17"/>
       <c r="R17" s="17"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="28" t="s">
         <v>22</v>
       </c>
@@ -1066,8 +1076,8 @@
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
       <c r="I18" s="18"/>
       <c r="J18" s="17"/>
       <c r="K18" s="17"/>
@@ -1079,7 +1089,7 @@
       <c r="Q18" s="17"/>
       <c r="R18" s="17"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
       <c r="D19" s="12" t="s">
@@ -1087,8 +1097,8 @@
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
       <c r="I19" s="18"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
@@ -1100,7 +1110,7 @@
       <c r="Q19" s="17"/>
       <c r="R19" s="17"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="12" t="s">
@@ -1108,8 +1118,8 @@
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33"/>
       <c r="I20" s="18"/>
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
@@ -1121,7 +1131,7 @@
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="28" t="s">
         <v>25</v>
       </c>
@@ -1131,8 +1141,8 @@
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
       <c r="I21" s="18"/>
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
@@ -1144,7 +1154,7 @@
       <c r="Q21" s="17"/>
       <c r="R21" s="17"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="12" t="s">
@@ -1152,8 +1162,8 @@
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="21"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33"/>
       <c r="I22" s="18"/>
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
@@ -1165,7 +1175,7 @@
       <c r="Q22" s="17"/>
       <c r="R22" s="17"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="12" t="s">
@@ -1173,8 +1183,8 @@
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33"/>
       <c r="I23" s="18"/>
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
@@ -1186,14 +1196,14 @@
       <c r="Q23" s="17"/>
       <c r="R23" s="17"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="2"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="35"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
       <c r="K24" s="17"/>
@@ -1205,7 +1215,7 @@
       <c r="Q24" s="17"/>
       <c r="R24" s="17"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="24" t="s">
         <v>2</v>
       </c>
@@ -1213,8 +1223,8 @@
       <c r="D25" s="9"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
       <c r="I25" s="20"/>
       <c r="J25" s="17"/>
       <c r="K25" s="17"/>
@@ -1226,7 +1236,7 @@
       <c r="Q25" s="17"/>
       <c r="R25" s="17"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
@@ -1234,8 +1244,8 @@
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="33"/>
       <c r="I26" s="18"/>
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
@@ -1247,7 +1257,7 @@
       <c r="Q26" s="17"/>
       <c r="R26" s="17"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9" t="s">
@@ -1255,8 +1265,8 @@
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="21"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
       <c r="I27" s="18"/>
       <c r="J27" s="17"/>
       <c r="K27" s="17"/>
@@ -1268,7 +1278,7 @@
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28" s="9" t="s">
@@ -1276,8 +1286,8 @@
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="33"/>
       <c r="I28" s="18"/>
       <c r="J28" s="17"/>
       <c r="K28" s="17"/>
@@ -1289,7 +1299,7 @@
       <c r="Q28" s="17"/>
       <c r="R28" s="17"/>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="D29" s="9" t="s">
@@ -1297,8 +1307,8 @@
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="30"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
       <c r="I29" s="18"/>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
@@ -1310,7 +1320,7 @@
       <c r="Q29" s="17"/>
       <c r="R29" s="17"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30" s="9" t="s">
@@ -1318,8 +1328,8 @@
       </c>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="30"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
       <c r="I30" s="18"/>
       <c r="J30" s="17"/>
       <c r="K30" s="17"/>
@@ -1331,7 +1341,7 @@
       <c r="Q30" s="17"/>
       <c r="R30" s="17"/>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31" s="9" t="s">
@@ -1339,8 +1349,8 @@
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="30"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
       <c r="I31" s="18"/>
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>
@@ -1352,7 +1362,7 @@
       <c r="Q31" s="17"/>
       <c r="R31" s="17"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="9" t="s">
@@ -1360,8 +1370,8 @@
       </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="33"/>
       <c r="I32" s="18"/>
       <c r="J32" s="17"/>
       <c r="K32" s="17"/>
@@ -1373,7 +1383,7 @@
       <c r="Q32" s="17"/>
       <c r="R32" s="17"/>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9" t="s">
@@ -1381,8 +1391,8 @@
       </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="33"/>
       <c r="I33" s="18"/>
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
@@ -1394,14 +1404,14 @@
       <c r="Q33" s="17"/>
       <c r="R33" s="17"/>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
       <c r="D34" s="2"/>
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="35"/>
       <c r="I34" s="20"/>
       <c r="J34" s="17"/>
       <c r="K34" s="17"/>
@@ -1413,17 +1423,17 @@
       <c r="Q34" s="17"/>
       <c r="R34" s="17"/>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="12"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="40"/>
       <c r="H35" s="41"/>
-      <c r="I35" s="39"/>
+      <c r="I35" s="31"/>
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
       <c r="L35" s="17"/>
@@ -1434,7 +1444,7 @@
       <c r="Q35" s="17"/>
       <c r="R35" s="17"/>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
       <c r="D36" s="12" t="s">
@@ -1442,8 +1452,8 @@
       </c>
       <c r="E36" s="18"/>
       <c r="F36" s="21"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="30"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
       <c r="I36" s="18"/>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
@@ -1455,7 +1465,7 @@
       <c r="Q36" s="17"/>
       <c r="R36" s="17"/>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
       <c r="D37" s="12" t="s">
@@ -1463,8 +1473,8 @@
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="21"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="30"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="37"/>
       <c r="I37" s="18"/>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
@@ -1476,7 +1486,7 @@
       <c r="Q37" s="17"/>
       <c r="R37" s="17"/>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
       <c r="D38" s="12" t="s">
@@ -1484,8 +1494,8 @@
       </c>
       <c r="E38" s="21"/>
       <c r="F38" s="21"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="30"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="37"/>
       <c r="I38" s="18"/>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
@@ -1497,7 +1507,7 @@
       <c r="Q38" s="17"/>
       <c r="R38" s="17"/>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
       <c r="D39" s="12" t="s">
@@ -1505,8 +1515,8 @@
       </c>
       <c r="E39" s="21"/>
       <c r="F39" s="21"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="30"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
       <c r="I39" s="18"/>
       <c r="J39" s="17"/>
       <c r="K39" s="17"/>
@@ -1518,7 +1528,7 @@
       <c r="Q39" s="17"/>
       <c r="R39" s="17"/>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
       <c r="D40" s="12" t="s">
@@ -1526,8 +1536,8 @@
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="21"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="30"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
       <c r="I40" s="18"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
@@ -1539,7 +1549,7 @@
       <c r="Q40" s="17"/>
       <c r="R40" s="17"/>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
       <c r="D41" s="12" t="s">
@@ -1547,8 +1557,8 @@
       </c>
       <c r="E41" s="18"/>
       <c r="F41" s="21"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="30"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
       <c r="I41" s="18"/>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
@@ -1560,7 +1570,7 @@
       <c r="Q41" s="17"/>
       <c r="R41" s="17"/>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
       <c r="D42" s="12" t="s">
@@ -1568,8 +1578,8 @@
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="21"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="30"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
       <c r="I42" s="18"/>
       <c r="J42" s="17"/>
       <c r="K42" s="17"/>
@@ -1581,7 +1591,7 @@
       <c r="Q42" s="17"/>
       <c r="R42" s="17"/>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
       <c r="D43" s="15" t="s">
@@ -1589,8 +1599,8 @@
       </c>
       <c r="E43" s="18"/>
       <c r="F43" s="21"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="30"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
       <c r="I43" s="18"/>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
@@ -1602,69 +1612,83 @@
       <c r="Q43" s="17"/>
       <c r="R43" s="17"/>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P44" s="16"/>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P45" s="16"/>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B46" s="19"/>
       <c r="D46" s="23" t="s">
         <v>42</v>
       </c>
       <c r="P46" s="16"/>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B47" s="22"/>
       <c r="D47" s="23" t="s">
         <v>43</v>
       </c>
       <c r="P47" s="16"/>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B48" s="35"/>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B48" s="29"/>
       <c r="D48" s="23" t="s">
         <v>44</v>
       </c>
       <c r="P48" s="16"/>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B49" s="36"/>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B49" s="30"/>
       <c r="D49" s="23" t="s">
         <v>45</v>
       </c>
       <c r="P49" s="16"/>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B50" s="42"/>
+      <c r="D50" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="P50" s="16"/>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P51" s="16"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P52" s="16"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P53" s="16"/>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P54" s="16"/>
     </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P55" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
@@ -1677,25 +1701,15 @@
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalised results for BiGUL
</commit_message>
<xml_diff>
--- a/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
+++ b/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
@@ -11,23 +11,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
-  <si>
-    <t>eMoflon</t>
-  </si>
-  <si>
-    <t>medini</t>
-  </si>
-  <si>
-    <t>medini (configurable)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+  <si>
+    <t xml:space="preserve">BiGul (state-based, runtime) </t>
+  </si>
+  <si>
+    <t>eMoflon (corr-based, structural-delta-based, runtime)</t>
+  </si>
+  <si>
+    <t>medini (corr-based, fixed)</t>
+  </si>
+  <si>
+    <t>medini (corr-based, runtime)</t>
   </si>
   <si>
     <t>Bxtend</t>
   </si>
   <si>
-    <t>BiGul</t>
-  </si>
-  <si>
     <t>Forward Batch</t>
   </si>
   <si>
@@ -103,7 +103,7 @@
     <t>IncrementalDeletions</t>
   </si>
   <si>
-    <t>due to missing OIDs</t>
+    <t>Although medini is corr-based, its trace model requires unique identifiers to work correctly in all cases</t>
   </si>
   <si>
     <t>IncrementalRename</t>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>IncrementalInsertsDynamicConfig</t>
+  </si>
+  <si>
+    <t>In the current BiGUL implementation, the assignment of people to families (which are just groups of names without roles in this phase) is separated from the assignment of members to their roles within each family.  This test, however, requires the first assignment to also take family roles into account, and will require a significant rewriting of the current implementation.</t>
   </si>
   <si>
     <t>Again least change: The rules are currently designed in such a way that empty families are deleted together with their last family member.  This is not trivial to fix, as handling families in a separate ignore rule would break the backward transformation, which requires such families (who would create them?)</t>
@@ -253,11 +256,11 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="14"/>
+      <color indexed="9"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,7 +269,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -290,6 +293,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="8"/>
         <bgColor auto="1"/>
       </patternFill>
@@ -300,8 +309,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -311,28 +326,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -341,16 +356,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -359,7 +374,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -369,7 +384,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -441,34 +456,8 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -476,43 +465,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -554,6 +513,36 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="8"/>
@@ -577,7 +566,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -587,7 +576,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -600,10 +589,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -613,29 +602,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,36 +639,32 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -689,203 +674,179 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -905,12 +866,13 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffd8d8d8"/>
       <rgbColor rgb="ff92d050"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff2600"/>
       <rgbColor rgb="ff4472c4"/>
     </indexedColors>
   </colors>
@@ -1110,17 +1072,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1148,10 +1110,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1399,12 +1361,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1691,7 +1653,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1719,10 +1681,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1973,7 +1935,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1982,22 +1944,13 @@
     <col min="1" max="1" width="10.8516" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.8516" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="48.3281" style="1" customWidth="1"/>
-    <col min="5" max="5" width="53" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.8516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.8516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.8516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.8516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.8516" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.8516" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.8516" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.8516" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.8516" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.8516" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.8516" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.8516" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.8516" style="1" customWidth="1"/>
-    <col min="19" max="256" width="10.8516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.4219" style="1" customWidth="1"/>
+    <col min="6" max="6" width="53" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.9297" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.1172" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1641" style="1" customWidth="1"/>
+    <col min="10" max="256" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -2010,15 +1963,6 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" s="2"/>
@@ -2030,15 +1974,6 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="4"/>
@@ -2054,1185 +1989,721 @@
       <c r="G3" t="s" s="8">
         <v>2</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" t="s" s="8">
+        <v>3</v>
+      </c>
       <c r="I3" t="s" s="8">
-        <v>3</v>
-      </c>
-      <c r="J3" t="s" s="8">
         <v>4</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="4"/>
-      <c r="B4" t="s" s="10">
+      <c r="B4" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" t="s" s="12">
+      <c r="C4" s="10"/>
+      <c r="D4" t="s" s="11">
         <v>6</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" s="4"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" t="s" s="12">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" t="s" s="11">
         <v>7</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" s="4"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" t="s" s="12">
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" t="s" s="11">
         <v>8</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" t="s" s="12">
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" t="s" s="11">
         <v>9</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" s="4"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" t="s" s="12">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" t="s" s="11">
         <v>10</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" s="4"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" t="s" s="12">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" t="s" s="11">
         <v>11</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="4"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" t="s" s="12">
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" t="s" s="11">
         <v>12</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" s="4"/>
-      <c r="B12" t="s" s="23">
+      <c r="B12" t="s" s="19">
         <v>13</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" s="4"/>
-      <c r="B13" t="s" s="26">
+      <c r="B13" t="s" s="22">
         <v>14</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" t="s" s="28">
+      <c r="C13" s="23"/>
+      <c r="D13" t="s" s="24">
         <v>15</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" s="4"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="27"/>
-      <c r="D14" t="s" s="28">
+      <c r="B14" s="25"/>
+      <c r="C14" s="23"/>
+      <c r="D14" t="s" s="24">
         <v>16</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" t="s" s="26">
+      <c r="B15" t="s" s="22">
         <v>17</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" t="s" s="28">
+      <c r="C15" s="23"/>
+      <c r="D15" t="s" s="24">
         <v>18</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" ht="15" customHeight="1">
       <c r="A16" s="4"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="27"/>
-      <c r="D16" t="s" s="28">
+      <c r="B16" s="25"/>
+      <c r="C16" s="23"/>
+      <c r="D16" t="s" s="24">
         <v>19</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" ht="15" customHeight="1">
       <c r="A17" s="4"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="27"/>
-      <c r="D17" t="s" s="28">
+      <c r="B17" s="25"/>
+      <c r="C17" s="23"/>
+      <c r="D17" t="s" s="24">
         <v>20</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" ht="15" customHeight="1">
       <c r="A18" s="4"/>
-      <c r="B18" t="s" s="26">
+      <c r="B18" t="s" s="22">
         <v>21</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" t="s" s="28">
+      <c r="C18" s="23"/>
+      <c r="D18" t="s" s="24">
         <v>15</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="A19" s="4"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="27"/>
-      <c r="D19" t="s" s="28">
+      <c r="B19" s="25"/>
+      <c r="C19" s="23"/>
+      <c r="D19" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" ht="15" customHeight="1">
       <c r="A20" s="4"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="27"/>
-      <c r="D20" t="s" s="28">
+      <c r="B20" s="25"/>
+      <c r="C20" s="23"/>
+      <c r="D20" t="s" s="24">
         <v>23</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="A21" s="4"/>
-      <c r="B21" t="s" s="26">
+      <c r="B21" t="s" s="22">
         <v>24</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" t="s" s="28">
+      <c r="C21" s="23"/>
+      <c r="D21" t="s" s="24">
         <v>18</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="A22" s="4"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="27"/>
-      <c r="D22" t="s" s="28">
+      <c r="B22" s="25"/>
+      <c r="C22" s="23"/>
+      <c r="D22" t="s" s="24">
         <v>25</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="A23" s="4"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="27"/>
-      <c r="D23" t="s" s="28">
+      <c r="B23" s="25"/>
+      <c r="C23" s="23"/>
+      <c r="D23" t="s" s="24">
         <v>26</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" ht="15" customHeight="1">
       <c r="A24" s="4"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
     </row>
     <row r="25" ht="15" customHeight="1">
       <c r="A25" s="4"/>
-      <c r="B25" t="s" s="10">
+      <c r="B25" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" ht="15" customHeight="1">
       <c r="A26" s="4"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" t="s" s="12">
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" t="s" s="11">
         <v>28</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-    </row>
-    <row r="27" ht="15" customHeight="1">
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" ht="51" customHeight="1">
       <c r="A27" s="4"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
-      <c r="D27" t="s" s="12">
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" t="s" s="28">
         <v>29</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="30"/>
-      <c r="G27" t="s" s="32">
+      <c r="E27" s="29"/>
+      <c r="F27" s="12"/>
+      <c r="G27" t="s" s="30">
         <v>30</v>
       </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
+      <c r="H27" t="s" s="30">
+        <v>30</v>
+      </c>
+      <c r="I27" s="12"/>
     </row>
     <row r="28" ht="15" customHeight="1">
       <c r="A28" s="4"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
-      <c r="D28" t="s" s="12">
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" t="s" s="11">
         <v>31</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" ht="80" customHeight="1">
       <c r="A29" s="4"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17"/>
-      <c r="D29" t="s" s="34">
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" t="s" s="28">
         <v>32</v>
       </c>
-      <c r="E29" t="s" s="35">
+      <c r="E29" s="29"/>
+      <c r="F29" t="s" s="31">
         <v>33</v>
       </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="12"/>
     </row>
     <row r="30" ht="80" customHeight="1">
       <c r="A30" s="4"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17"/>
-      <c r="D30" t="s" s="34">
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
+      <c r="D30" t="s" s="28">
         <v>34</v>
       </c>
-      <c r="E30" t="s" s="35">
+      <c r="E30" s="29"/>
+      <c r="F30" t="s" s="31">
         <v>35</v>
       </c>
-      <c r="F30" s="30"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" ht="15" customHeight="1">
       <c r="A31" s="4"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17"/>
-      <c r="D31" t="s" s="12">
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="D31" t="s" s="11">
         <v>36</v>
       </c>
-      <c r="E31" t="s" s="37">
+      <c r="E31" s="29"/>
+      <c r="F31" t="s" s="32">
         <v>37</v>
       </c>
-      <c r="F31" s="30"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="12"/>
     </row>
     <row r="32" ht="15" customHeight="1">
       <c r="A32" s="4"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17"/>
-      <c r="D32" t="s" s="12">
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
+      <c r="D32" t="s" s="11">
         <v>38</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
     </row>
     <row r="33" ht="15" customHeight="1">
       <c r="A33" s="4"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
-      <c r="D33" t="s" s="12">
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
+      <c r="D33" t="s" s="11">
         <v>39</v>
       </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
     </row>
     <row r="34" ht="15" customHeight="1">
       <c r="A34" s="4"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="9"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" ht="15" customHeight="1">
       <c r="A35" s="4"/>
-      <c r="B35" t="s" s="23">
+      <c r="B35" t="s" s="19">
         <v>40</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="A36" s="4"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="27"/>
-      <c r="D36" t="s" s="28">
+      <c r="B36" s="25"/>
+      <c r="C36" s="23"/>
+      <c r="D36" t="s" s="24">
         <v>41</v>
       </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-    </row>
-    <row r="37" ht="15" customHeight="1">
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" ht="102" customHeight="1">
       <c r="A37" s="4"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="27"/>
-      <c r="D37" t="s" s="28">
+      <c r="B37" s="25"/>
+      <c r="C37" s="23"/>
+      <c r="D37" t="s" s="33">
         <v>42</v>
       </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
+      <c r="E37" t="s" s="34">
+        <v>43</v>
+      </c>
+      <c r="F37" s="12"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="12"/>
     </row>
     <row r="38" ht="58" customHeight="1">
       <c r="A38" s="4"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="27"/>
-      <c r="D38" t="s" s="38">
+      <c r="B38" s="25"/>
+      <c r="C38" s="23"/>
+      <c r="D38" t="s" s="33">
         <v>29</v>
       </c>
-      <c r="E38" t="s" s="35">
-        <v>43</v>
-      </c>
-      <c r="F38" s="30"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
-      <c r="R38" s="9"/>
+      <c r="E38" s="12"/>
+      <c r="F38" t="s" s="31">
+        <v>44</v>
+      </c>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="12"/>
     </row>
     <row r="39" ht="69" customHeight="1">
       <c r="A39" s="4"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="27"/>
-      <c r="D39" t="s" s="38">
-        <v>44</v>
-      </c>
-      <c r="E39" t="s" s="35">
+      <c r="B39" s="25"/>
+      <c r="C39" s="23"/>
+      <c r="D39" t="s" s="33">
         <v>45</v>
       </c>
-      <c r="F39" s="30"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
+      <c r="E39" s="29"/>
+      <c r="F39" t="s" s="31">
+        <v>46</v>
+      </c>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" ht="15" customHeight="1">
       <c r="A40" s="4"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="27"/>
-      <c r="D40" t="s" s="28">
-        <v>46</v>
-      </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="9"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="23"/>
+      <c r="D40" t="s" s="24">
+        <v>47</v>
+      </c>
+      <c r="E40" s="29"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="12"/>
     </row>
     <row r="41" ht="25" customHeight="1">
       <c r="A41" s="4"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="27"/>
-      <c r="D41" t="s" s="38">
-        <v>47</v>
-      </c>
-      <c r="E41" t="s" s="39">
+      <c r="B41" s="25"/>
+      <c r="C41" s="23"/>
+      <c r="D41" t="s" s="33">
         <v>48</v>
       </c>
-      <c r="F41" s="40"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
+      <c r="E41" s="29"/>
+      <c r="F41" t="s" s="35">
+        <v>49</v>
+      </c>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="12"/>
     </row>
     <row r="42" ht="15" customHeight="1">
       <c r="A42" s="4"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="27"/>
-      <c r="D42" t="s" s="28">
+      <c r="B42" s="25"/>
+      <c r="C42" s="23"/>
+      <c r="D42" t="s" s="24">
         <v>38</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="9"/>
-      <c r="R42" s="9"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="12"/>
     </row>
     <row r="43" ht="15" customHeight="1">
       <c r="A43" s="4"/>
-      <c r="B43" s="42"/>
-      <c r="C43" s="43"/>
-      <c r="D43" t="s" s="44">
+      <c r="B43" s="36"/>
+      <c r="C43" s="37"/>
+      <c r="D43" t="s" s="38">
         <v>39</v>
       </c>
-      <c r="E43" s="13"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" ht="15" customHeight="1">
       <c r="A44" s="4"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="18"/>
     </row>
     <row r="45" ht="15" customHeight="1">
       <c r="A45" s="4"/>
-      <c r="B45" t="s" s="47">
-        <v>49</v>
-      </c>
-      <c r="C45" s="48"/>
-      <c r="D45" t="s" s="49">
+      <c r="B45" t="s" s="42">
         <v>50</v>
       </c>
-      <c r="E45" s="9">
+      <c r="C45" s="43"/>
+      <c r="D45" t="s" s="44">
+        <v>51</v>
+      </c>
+      <c r="E45" s="18">
+        <v>176</v>
+      </c>
+      <c r="F45" s="18">
         <v>157</v>
       </c>
-      <c r="F45" s="9">
+      <c r="G45" s="18">
         <v>157</v>
       </c>
-      <c r="G45" s="21">
+      <c r="H45" s="18">
         <v>320</v>
       </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="9">
+      <c r="I45" s="18">
         <v>211</v>
       </c>
-      <c r="J45" s="9">
-        <v>181</v>
-      </c>
-      <c r="K45" s="9"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9"/>
-      <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
     </row>
     <row r="46" ht="15" customHeight="1">
       <c r="A46" s="4"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="24"/>
-      <c r="D46" t="s" s="28">
-        <v>51</v>
-      </c>
-      <c r="E46" s="9">
+      <c r="B46" s="45"/>
+      <c r="C46" s="20"/>
+      <c r="D46" t="s" s="24">
+        <v>52</v>
+      </c>
+      <c r="E46" s="18">
+        <v>853</v>
+      </c>
+      <c r="F46" s="18">
         <v>255</v>
       </c>
-      <c r="F46" s="9">
+      <c r="G46" s="18">
         <v>515</v>
       </c>
-      <c r="G46" s="21">
+      <c r="H46" s="18">
         <v>956</v>
       </c>
-      <c r="H46" s="22"/>
-      <c r="I46" s="9">
+      <c r="I46" s="18">
         <v>565</v>
       </c>
-      <c r="J46" s="9">
-        <v>710</v>
-      </c>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
     </row>
     <row r="47" ht="15" customHeight="1">
       <c r="A47" s="4"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="24"/>
-      <c r="D47" t="s" s="44">
-        <v>52</v>
-      </c>
-      <c r="E47" s="9">
+      <c r="B47" s="45"/>
+      <c r="C47" s="20"/>
+      <c r="D47" t="s" s="38">
+        <v>53</v>
+      </c>
+      <c r="E47" s="18">
+        <v>8325</v>
+      </c>
+      <c r="F47" s="18">
         <v>2795</v>
       </c>
-      <c r="F47" s="9">
+      <c r="G47" s="18">
         <v>4035</v>
       </c>
-      <c r="G47" s="21">
+      <c r="H47" s="18">
         <v>9740</v>
       </c>
-      <c r="H47" s="22"/>
-      <c r="I47" s="9">
+      <c r="I47" s="18">
         <v>7571</v>
       </c>
-      <c r="J47" s="9">
-        <v>6629</v>
-      </c>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="9"/>
-      <c r="R47" s="9"/>
     </row>
     <row r="48" ht="15" customHeight="1">
       <c r="A48" s="4"/>
-      <c r="B48" s="51"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
-      <c r="O48" s="9"/>
-      <c r="P48" s="9"/>
-      <c r="Q48" s="9"/>
-      <c r="R48" s="9"/>
+      <c r="B48" s="46"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="A49" s="2"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="54"/>
-      <c r="G49" s="54"/>
-      <c r="H49" s="54"/>
-      <c r="I49" s="54"/>
-      <c r="J49" s="54"/>
-      <c r="K49" s="54"/>
-      <c r="L49" s="54"/>
-      <c r="M49" s="54"/>
-      <c r="N49" s="54"/>
-      <c r="O49" s="54"/>
-      <c r="P49" s="55"/>
-      <c r="Q49" s="54"/>
-      <c r="R49" s="54"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="49"/>
     </row>
     <row r="50" ht="15" customHeight="1">
-      <c r="A50" s="56"/>
-      <c r="B50" s="57"/>
-      <c r="C50" s="58"/>
-      <c r="D50" t="s" s="59">
-        <v>53</v>
-      </c>
-      <c r="E50" s="60"/>
+      <c r="A50" s="50"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="52"/>
+      <c r="D50" t="s" s="53">
+        <v>54</v>
+      </c>
+      <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="61"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
     </row>
     <row r="51" ht="15" customHeight="1">
-      <c r="A51" s="56"/>
-      <c r="B51" s="62"/>
-      <c r="C51" s="58"/>
-      <c r="D51" t="s" s="59">
-        <v>54</v>
-      </c>
-      <c r="E51" s="60"/>
+      <c r="A51" s="50"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="52"/>
+      <c r="D51" t="s" s="53">
+        <v>55</v>
+      </c>
+      <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
-      <c r="P51" s="61"/>
-      <c r="Q51" s="2"/>
-      <c r="R51" s="2"/>
     </row>
     <row r="52" ht="15" customHeight="1">
-      <c r="A52" s="56"/>
-      <c r="B52" s="63"/>
-      <c r="C52" s="58"/>
-      <c r="D52" t="s" s="59">
-        <v>55</v>
-      </c>
-      <c r="E52" s="60"/>
+      <c r="A52" s="50"/>
+      <c r="B52" s="55"/>
+      <c r="C52" s="52"/>
+      <c r="D52" t="s" s="53">
+        <v>56</v>
+      </c>
+      <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="61"/>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="2"/>
     </row>
     <row r="53" ht="15" customHeight="1">
-      <c r="A53" s="56"/>
-      <c r="B53" s="64"/>
-      <c r="C53" s="58"/>
-      <c r="D53" t="s" s="59">
-        <v>56</v>
-      </c>
-      <c r="E53" s="60"/>
+      <c r="A53" s="50"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="52"/>
+      <c r="D53" t="s" s="53">
+        <v>57</v>
+      </c>
+      <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="61"/>
-      <c r="Q53" s="2"/>
-      <c r="R53" s="2"/>
     </row>
     <row r="54" ht="15" customHeight="1">
       <c r="A54" s="2"/>
-      <c r="B54" s="65"/>
+      <c r="B54" s="57"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="65"/>
+      <c r="D54" s="57"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
-      <c r="P54" s="61"/>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
     </row>
     <row r="55" ht="15" customHeight="1">
       <c r="A55" s="2"/>
@@ -3244,64 +2715,8 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-      <c r="O55" s="2"/>
-      <c r="P55" s="61"/>
-      <c r="Q55" s="2"/>
-      <c r="R55" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G44:H44"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
Adapt metrics in excel sheet
</commit_message>
<xml_diff>
--- a/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
+++ b/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
@@ -470,7 +470,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -654,7 +654,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
+      <selection pane="topLeft" activeCell="J48" activeCellId="0" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1365,7 +1365,7 @@
         <v>211</v>
       </c>
       <c r="J45" s="1" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1391,7 +1391,7 @@
         <v>565</v>
       </c>
       <c r="J46" s="1" t="n">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1417,7 +1417,7 @@
         <v>7571</v>
       </c>
       <c r="J47" s="1" t="n">
-        <v>2040</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Small change in excel sheet
</commit_message>
<xml_diff>
--- a/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
+++ b/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Bxtend</t>
   </si>
   <si>
-    <t xml:space="preserve">FunnyQT (state-based)</t>
+    <t xml:space="preserve">FunnyQT (state-based, runtime)</t>
   </si>
   <si>
     <t xml:space="preserve">Forward Batch</t>
@@ -653,8 +653,8 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J48" activeCellId="0" sqref="J48"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Final update to FunnyQT solution
</commit_message>
<xml_diff>
--- a/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
+++ b/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
@@ -653,8 +653,8 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J48" activeCellId="0" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1365,7 +1365,7 @@
         <v>211</v>
       </c>
       <c r="J45" s="1" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1417,7 +1417,7 @@
         <v>7571</v>
       </c>
       <c r="J47" s="1" t="n">
-        <v>2098</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Final update to FunnyQT solution (#49)
</commit_message>
<xml_diff>
--- a/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
+++ b/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
@@ -653,8 +653,8 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J48" activeCellId="0" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1365,7 +1365,7 @@
         <v>211</v>
       </c>
       <c r="J45" s="1" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1417,7 +1417,7 @@
         <v>7571</v>
       </c>
       <c r="J47" s="1" t="n">
-        <v>2098</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix a bug in FunnyQT solution; now only 9 tests failing
</commit_message>
<xml_diff>
--- a/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
+++ b/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t xml:space="preserve">BiGul (state-based, runtime) </t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">initialize</t>
   </si>
   <si>
-    <t xml:space="preserve">All tests passed</t>
+    <t xml:space="preserve">All expected passes</t>
   </si>
   <si>
     <t xml:space="preserve">changeEmptyFamily</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">IncrementalInserts</t>
   </si>
   <si>
-    <t xml:space="preserve">passed</t>
+    <t xml:space="preserve">expected pass</t>
   </si>
   <si>
     <t xml:space="preserve">IncrementalDeletions</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Although medini is corr-based, its trace model requires unique identifiers to work correctly in all cases</t>
   </si>
   <si>
-    <t xml:space="preserve">failed</t>
+    <t xml:space="preserve">expected fail</t>
   </si>
   <si>
     <t xml:space="preserve">IncrementalRename</t>
@@ -184,6 +184,9 @@
     <t xml:space="preserve">In the current BiGUL implementation, the assignment of people to families (which are just groups of names without roles in this phase) is separated from the assignment of members to their roles within each family.  This test, however, requires the first assignment to also take family roles into account, and will require a significant rewriting of the current implementation.</t>
   </si>
   <si>
+    <t xml:space="preserve">unexpected fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">Again least change: The rules are currently designed in such a way that empty families are deleted together with their last family member.  This is not trivial to fix, as handling families in a separate ignore rule would break the backward transformation, which requires such families (who would create them?)</t>
   </si>
   <si>
@@ -226,7 +229,7 @@
     <t xml:space="preserve">Limitation</t>
   </si>
   <si>
-    <t xml:space="preserve">FunnyQT’s BX-transformation framework is essentially state-based although it is possible to feed the trace from one run of the transformation into the next run.  However, that works only if elements have some kind of identity so I implemented the simplest solution that works correctly for at least the batch cases.</t>
+    <t xml:space="preserve">FunnyQT’s BX-transformation framework is essentially state-based and not incremental (listening to model changes) and doesn’t preserve correspondences between transformation executions, so operations like renaming or moving are resolved by deletion and re-creation which might loose information manually set in the target model (like the birthdays).</t>
   </si>
 </sst>
 </file>
@@ -653,8 +656,10 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J48" activeCellId="0" sqref="J48"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="0" topLeftCell="I46" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+      <selection pane="topRight" activeCell="J54" activeCellId="0" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1224,7 +1229,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="16" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="58" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1236,7 +1241,7 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -1250,11 +1255,11 @@
       <c r="B39" s="9"/>
       <c r="C39" s="10"/>
       <c r="D39" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -1268,7 +1273,7 @@
       <c r="B40" s="9"/>
       <c r="C40" s="10"/>
       <c r="D40" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1284,17 +1289,17 @@
       <c r="B41" s="9"/>
       <c r="C41" s="10"/>
       <c r="D41" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="16" t="s">
-        <v>34</v>
+      <c r="J41" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1343,11 +1348,11 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C45" s="25"/>
       <c r="D45" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E45" s="2" t="n">
         <v>176</v>
@@ -1365,7 +1370,7 @@
         <v>211</v>
       </c>
       <c r="J45" s="1" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1373,7 +1378,7 @@
       <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E46" s="2" t="n">
         <v>853</v>
@@ -1391,7 +1396,7 @@
         <v>565</v>
       </c>
       <c r="J46" s="1" t="n">
-        <v>246</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1399,7 +1404,7 @@
       <c r="B47" s="27"/>
       <c r="C47" s="6"/>
       <c r="D47" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E47" s="2" t="n">
         <v>8325</v>
@@ -1417,7 +1422,7 @@
         <v>7571</v>
       </c>
       <c r="J47" s="1" t="n">
-        <v>2034</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1447,7 +1452,7 @@
       <c r="B50" s="30"/>
       <c r="C50" s="31"/>
       <c r="D50" s="32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -1460,7 +1465,7 @@
       <c r="B51" s="30"/>
       <c r="C51" s="31"/>
       <c r="D51" s="32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -1473,7 +1478,7 @@
       <c r="B52" s="30"/>
       <c r="C52" s="31"/>
       <c r="D52" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
@@ -1481,12 +1486,12 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="131.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="161.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="29"/>
       <c r="B53" s="30"/>
       <c r="C53" s="31"/>
       <c r="D53" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -1494,7 +1499,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix a bug in FunnyQT solution; now only 9 tests failing (#53)
</commit_message>
<xml_diff>
--- a/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
+++ b/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t xml:space="preserve">BiGul (state-based, runtime) </t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">initialize</t>
   </si>
   <si>
-    <t xml:space="preserve">All tests passed</t>
+    <t xml:space="preserve">All expected passes</t>
   </si>
   <si>
     <t xml:space="preserve">changeEmptyFamily</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">IncrementalInserts</t>
   </si>
   <si>
-    <t xml:space="preserve">passed</t>
+    <t xml:space="preserve">expected pass</t>
   </si>
   <si>
     <t xml:space="preserve">IncrementalDeletions</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Although medini is corr-based, its trace model requires unique identifiers to work correctly in all cases</t>
   </si>
   <si>
-    <t xml:space="preserve">failed</t>
+    <t xml:space="preserve">expected fail</t>
   </si>
   <si>
     <t xml:space="preserve">IncrementalRename</t>
@@ -184,6 +184,9 @@
     <t xml:space="preserve">In the current BiGUL implementation, the assignment of people to families (which are just groups of names without roles in this phase) is separated from the assignment of members to their roles within each family.  This test, however, requires the first assignment to also take family roles into account, and will require a significant rewriting of the current implementation.</t>
   </si>
   <si>
+    <t xml:space="preserve">unexpected fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">Again least change: The rules are currently designed in such a way that empty families are deleted together with their last family member.  This is not trivial to fix, as handling families in a separate ignore rule would break the backward transformation, which requires such families (who would create them?)</t>
   </si>
   <si>
@@ -226,7 +229,7 @@
     <t xml:space="preserve">Limitation</t>
   </si>
   <si>
-    <t xml:space="preserve">FunnyQT’s BX-transformation framework is essentially state-based although it is possible to feed the trace from one run of the transformation into the next run.  However, that works only if elements have some kind of identity so I implemented the simplest solution that works correctly for at least the batch cases.</t>
+    <t xml:space="preserve">FunnyQT’s BX-transformation framework is essentially state-based and not incremental (listening to model changes) and doesn’t preserve correspondences between transformation executions, so operations like renaming or moving are resolved by deletion and re-creation which might loose information manually set in the target model (like the birthdays).</t>
   </si>
 </sst>
 </file>
@@ -653,8 +656,10 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J48" activeCellId="0" sqref="J48"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="0" topLeftCell="I46" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+      <selection pane="topRight" activeCell="J54" activeCellId="0" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1224,7 +1229,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="16" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="58" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1236,7 +1241,7 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -1250,11 +1255,11 @@
       <c r="B39" s="9"/>
       <c r="C39" s="10"/>
       <c r="D39" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -1268,7 +1273,7 @@
       <c r="B40" s="9"/>
       <c r="C40" s="10"/>
       <c r="D40" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1284,17 +1289,17 @@
       <c r="B41" s="9"/>
       <c r="C41" s="10"/>
       <c r="D41" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="16" t="s">
-        <v>34</v>
+      <c r="J41" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1343,11 +1348,11 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C45" s="25"/>
       <c r="D45" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E45" s="2" t="n">
         <v>176</v>
@@ -1365,7 +1370,7 @@
         <v>211</v>
       </c>
       <c r="J45" s="1" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1373,7 +1378,7 @@
       <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E46" s="2" t="n">
         <v>853</v>
@@ -1391,7 +1396,7 @@
         <v>565</v>
       </c>
       <c r="J46" s="1" t="n">
-        <v>246</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1399,7 +1404,7 @@
       <c r="B47" s="27"/>
       <c r="C47" s="6"/>
       <c r="D47" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E47" s="2" t="n">
         <v>8325</v>
@@ -1417,7 +1422,7 @@
         <v>7571</v>
       </c>
       <c r="J47" s="1" t="n">
-        <v>2034</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1447,7 +1452,7 @@
       <c r="B50" s="30"/>
       <c r="C50" s="31"/>
       <c r="D50" s="32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -1460,7 +1465,7 @@
       <c r="B51" s="30"/>
       <c r="C51" s="31"/>
       <c r="D51" s="32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -1473,7 +1478,7 @@
       <c r="B52" s="30"/>
       <c r="C52" s="31"/>
       <c r="D52" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
@@ -1481,12 +1486,12 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="131.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="161.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="29"/>
       <c r="B53" s="30"/>
       <c r="C53" s="31"/>
       <c r="D53" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -1494,7 +1499,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed a three test cases for the NMF solution
</commit_message>
<xml_diff>
--- a/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
+++ b/examples/familiestopersons/BenchmarxFamiliesToPersons/results/TestResults.xlsx
@@ -217,13 +217,13 @@
     <t>NMF (incremental, runtime)</t>
   </si>
   <si>
-    <t>In all of these failures, I actually do not understand the "spec". The transformation produces exactly the intended behavior, the failures is because I do not understand the semantics of the configurations.</t>
-  </si>
-  <si>
     <t>The solution does not detect a move</t>
   </si>
   <si>
     <t>FunnyQT’s BX-transformation framework is essentially state-based and not incremental (listening to model changes) and doesn’t preserve correspondences between transformation executions, so operations like renaming or moving are resolved by deletion and re-creation which might loose information manually set in the target model (like the birthdays).</t>
+  </si>
+  <si>
+    <t>Rename somehow currently does not work</t>
   </si>
 </sst>
 </file>
@@ -1952,8 +1952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E31" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E34" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="I27" s="12"/>
       <c r="J27" s="62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K27" s="12"/>
     </row>
@@ -2426,7 +2426,7 @@
       <c r="I29" s="12"/>
       <c r="J29" s="63"/>
       <c r="K29" s="61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -2462,7 +2462,7 @@
       <c r="I31" s="12"/>
       <c r="J31" s="64"/>
       <c r="K31" s="61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2536,7 +2536,7 @@
       <c r="H36" s="26"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
-      <c r="K36" s="58"/>
+      <c r="K36" s="12"/>
     </row>
     <row r="37" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
@@ -2553,9 +2553,7 @@
       <c r="H37" s="26"/>
       <c r="I37" s="12"/>
       <c r="J37" s="58"/>
-      <c r="K37" s="60" t="s">
-        <v>60</v>
-      </c>
+      <c r="K37" s="12"/>
     </row>
     <row r="38" spans="1:11" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
@@ -2589,7 +2587,9 @@
       <c r="H39" s="26"/>
       <c r="I39" s="12"/>
       <c r="J39" s="59"/>
-      <c r="K39" s="58"/>
+      <c r="K39" s="60" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
@@ -2621,7 +2621,7 @@
       <c r="H41" s="29"/>
       <c r="I41" s="12"/>
       <c r="J41" s="59"/>
-      <c r="K41" s="58"/>
+      <c r="K41" s="12"/>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
@@ -2694,7 +2694,7 @@
         <v>52</v>
       </c>
       <c r="K45" s="18">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2723,7 +2723,7 @@
         <v>264</v>
       </c>
       <c r="K46" s="18">
-        <v>524</v>
+        <v>436</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2752,7 +2752,7 @@
         <v>2172</v>
       </c>
       <c r="K47" s="18">
-        <v>4492</v>
+        <v>4392</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>